<commit_message>
Modfiy Excel Templates Date
</commit_message>
<xml_diff>
--- a/dreamwedding/templates/admin/excel_templates/导入模板.xlsx
+++ b/dreamwedding/templates/admin/excel_templates/导入模板.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>红色字体勿动</t>
   </si>
@@ -33,20 +33,39 @@
     <t>状态</t>
   </si>
   <si>
+    <t>刻盘日期（日期格式为：xxxx/xx/xx）</t>
+  </si>
+  <si>
     <t>备注</t>
+  </si>
+  <si>
+    <t>A171945</t>
+  </si>
+  <si>
+    <t>测试</t>
+  </si>
+  <si>
+    <t>已完成</t>
+  </si>
+  <si>
+    <t>A171905</t>
+  </si>
+  <si>
+    <t>D6854</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +97,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -94,30 +136,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -126,7 +160,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -140,7 +174,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -155,7 +189,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,60 +197,38 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,19 +243,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -255,13 +381,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,145 +423,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,11 +437,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -449,6 +467,33 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -464,17 +509,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -493,197 +534,171 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1033,46 +1048,99 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="5" width="15.625" customWidth="1"/>
+    <col min="1" max="4" width="15.625" customWidth="1"/>
+    <col min="5" max="5" width="41.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:5">
+    <row r="1" ht="25" customHeight="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
-    <row r="2" ht="25" customHeight="1" spans="1:5">
-      <c r="A2" s="3" t="s">
+    <row r="2" ht="25" customHeight="1" spans="1:6">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" ht="25" customHeight="1"/>
-    <row r="4" ht="25" customHeight="1"/>
-    <row r="5" ht="25" customHeight="1"/>
+    <row r="3" ht="25" customHeight="1" spans="1:5">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4">
+        <v>43541</v>
+      </c>
+    </row>
+    <row r="4" ht="25" customHeight="1" spans="1:5">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4">
+        <v>43543</v>
+      </c>
+    </row>
+    <row r="5" ht="25" customHeight="1" spans="1:5">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4">
+        <v>43544</v>
+      </c>
+    </row>
     <row r="6" ht="25" customHeight="1"/>
     <row r="7" ht="25" customHeight="1"/>
     <row r="8" ht="25" customHeight="1"/>
@@ -1095,7 +1163,7 @@
     <row r="25" ht="25" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>